<commit_message>
updated data from niraqa
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/doc_category.xlsx
+++ b/mosip_master/xlsx/doc_category.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karthik.SJ\Documents\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tf_nira\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417D99BD-B784-4BD6-9AE3-CB5D6B4852A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FCF303-F463-416D-A83D-89FEDAC654E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F7CCF4D-8218-47FF-82F6-EB07A560EBA0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F7CCF4D-8218-47FF-82F6-EB07A560EBA0}"/>
   </bookViews>
   <sheets>
     <sheet name="doc_category" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="85">
   <si>
     <t>code</t>
   </si>
@@ -263,13 +263,28 @@
   </si>
   <si>
     <t>Proof of other supporting document</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>Proof of Loss</t>
+  </si>
+  <si>
+    <t>POPF</t>
+  </si>
+  <si>
+    <t>Proof of Physical Application Form</t>
+  </si>
+  <si>
+    <t>Proof of Physical Application Form (Required for Walk-In Applications)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +415,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -746,10 +768,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1125,21 +1149,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FAEBCC2-B773-4107-AFE8-13DD4FA99942}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1174,7 +1198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1206,7 +1230,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1238,7 +1262,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1270,7 +1294,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1302,7 +1326,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1334,7 +1358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1366,7 +1390,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1398,7 +1422,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1430,7 +1454,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1462,7 +1486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1494,7 +1518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1526,7 +1550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1558,7 +1582,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1590,7 +1614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1622,7 +1646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1654,7 +1678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1686,7 +1710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -1718,7 +1742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1750,7 +1774,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -1782,7 +1806,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1814,7 +1838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1846,7 +1870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -1878,7 +1902,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1910,7 +1934,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1942,7 +1966,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1974,7 +1998,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -2006,7 +2030,103 @@
         <v>17</v>
       </c>
     </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="1">
+        <v>45516.749305555553</v>
+      </c>
+      <c r="J28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="1">
+        <v>45516.749305555553</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="1">
+        <v>45516.749305555553</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="1">
+        <v>45516.749305555553</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>